<commit_message>
change more case write_data commit
</commit_message>
<xml_diff>
--- a/Data/api_test.xlsx
+++ b/Data/api_test.xlsx
@@ -8,15 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="allure报告打开方式" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="75">
   <si>
     <t>用例编号</t>
   </si>
@@ -129,7 +128,7 @@
     <t>queryTrafficAvg（日均流量消耗）</t>
   </si>
   <si>
-    <t>http://test1.boxingtong.net:5222/analyse/dashboard/queryTrafficAv</t>
+    <t>http://test1.boxingtong.net:5222/analyse/dashboard/queryTrafficAvg</t>
   </si>
   <si>
     <t>bxt_api_005</t>
@@ -177,31 +176,105 @@
     <t>http://test1.boxingtong.net:5222/analyse/dashboard/queryShipToZoo</t>
   </si>
   <si>
-    <t>步骤1</t>
-  </si>
-  <si>
-    <t>分别解压allure.zip,html.zip到本地任意路径</t>
-  </si>
-  <si>
-    <t>步骤2</t>
-  </si>
-  <si>
-    <t>右键我的电脑-属性-高级系统设置-环境变量-系统变量，找到Path(不区分大小写），双击编辑，把allure解压后的bin目录添加到path中，例如：D:\allure-2.14.0\bin</t>
-  </si>
-  <si>
-    <t>步骤3</t>
-  </si>
-  <si>
-    <t>打开dos窗口，输入CMD，确定，进入命令行，输入allure --version.出现版本号即环境变量设置成功。</t>
-  </si>
-  <si>
-    <t>步骤4</t>
-  </si>
-  <si>
-    <t>输入命令allure open -h 127.0.0.1 -p8686 D:\html(本机ip+任意端口号+html解压路径）即可打开报告</t>
-  </si>
-  <si>
-    <t>allure环境变量配置完成之后，后续不需要再次配置，直接在DOS窗口输入打开报告的命令就可以。</t>
+    <t>bxt_app_api_001</t>
+  </si>
+  <si>
+    <t>波星通APP</t>
+  </si>
+  <si>
+    <t>首页</t>
+  </si>
+  <si>
+    <t>奖励记录列表</t>
+  </si>
+  <si>
+    <t>http://test1.boxingtong.net:9001/reward/selectRewardRecordList</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>{
+ "code":1,
+ "data":{
+},
+ "message":"操作成功！"
+}</t>
+  </si>
+  <si>
+    <t>bxt_app_api_002</t>
+  </si>
+  <si>
+    <t>奖励banner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+http://test1.boxingtong.net:9001/reward/isShowBanner</t>
+  </si>
+  <si>
+    <t>bxt_app_api_003</t>
+  </si>
+  <si>
+    <t>VIP弹窗</t>
+  </si>
+  <si>
+    <t>http://test1.boxingtong.net:9001/account/getVIPPopup</t>
+  </si>
+  <si>
+    <t>bxt_app_api_004</t>
+  </si>
+  <si>
+    <t>banner列表</t>
+  </si>
+  <si>
+    <t>http://test1.boxingtong.net:8001/banner/selectBanner</t>
+  </si>
+  <si>
+    <t>{"sdkVersionCode":29}</t>
+  </si>
+  <si>
+    <t>bxt_app_api_005</t>
+  </si>
+  <si>
+    <t>昨日流量消耗记录</t>
+  </si>
+  <si>
+    <t>http://test1.boxingtong.net:8001/consume/queryCurrentUsage</t>
+  </si>
+  <si>
+    <t>bxt_app_api_006</t>
+  </si>
+  <si>
+    <t>可用波呗</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+http://test1.boxingtong.net:8001/account/getAccountInfo</t>
+  </si>
+  <si>
+    <t>bxt_app_api_007</t>
+  </si>
+  <si>
+    <t>首页弹窗</t>
+  </si>
+  <si>
+    <t>http://test1.boxingtong.net:8001/banner/selectHomePopup</t>
+  </si>
+  <si>
+    <t>bxt_app_api_008</t>
+  </si>
+  <si>
+    <t>版本更新详情</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+http://test1.boxingtong.net:8001/share/app/appUpdateByPackage</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>{"packageName":"com.bird.fisher","version":"3.5.0"}</t>
   </si>
 </sst>
 </file>
@@ -209,15 +282,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -238,16 +319,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,17 +371,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -282,8 +386,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -298,39 +403,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -382,7 +455,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,7 +464,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,79 +530,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,85 +620,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -588,6 +655,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -631,30 +722,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -696,10 +763,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -708,73 +775,73 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -783,90 +850,96 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -928,125 +1001,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2430780</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>6225540</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1625600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1" descr="1648531748(1)"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3048000" y="899160"/>
-          <a:ext cx="6263640" cy="1488440"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>67945</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3528060</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2" descr="1648531785(1)"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3093720" y="2798445"/>
-          <a:ext cx="3520440" cy="1468755"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>124460</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>4953635</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>1005840</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="图片 3" descr="1648531825(1)"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3093720" y="4353560"/>
-          <a:ext cx="4946015" cy="881380"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1338,21 +1292,21 @@
   <sheetPr/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="3" width="18.3333333333333" customWidth="1"/>
-    <col min="4" max="4" width="20" style="3" customWidth="1"/>
-    <col min="5" max="6" width="26.3333333333333" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.2222222222222" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="1" customWidth="1"/>
+    <col min="5" max="6" width="26.3333333333333" style="6" customWidth="1"/>
+    <col min="7" max="7" width="26.2222222222222" style="6" customWidth="1"/>
+    <col min="8" max="8" width="34" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36" customHeight="1" spans="1:8">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1361,23 +1315,23 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="208.95" customHeight="1" spans="1:8">
+    <row r="2" ht="302.4" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1387,23 +1341,23 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" ht="249" customHeight="1" spans="1:8">
+    <row r="3" ht="129" customHeight="1" spans="1:8">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1413,23 +1367,23 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" ht="86.4" spans="1:8">
+    <row r="4" ht="85" customHeight="1" spans="1:8">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1439,23 +1393,23 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" ht="129" customHeight="1" spans="1:8">
+    <row r="5" ht="97" customHeight="1" spans="1:8">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1465,23 +1419,23 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" ht="85" customHeight="1" spans="1:8">
+    <row r="6" ht="97" customHeight="1" spans="1:8">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1491,19 +1445,19 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1517,19 +1471,19 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1543,23 +1497,23 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" ht="97" customHeight="1" spans="1:8">
+    <row r="9" ht="86.4" spans="1:8">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1569,23 +1523,23 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" ht="97" customHeight="1" spans="1:8">
+    <row r="10" ht="86.4" spans="1:8">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1595,19 +1549,19 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1616,7 +1570,7 @@
     <hyperlink ref="E2" r:id="rId1" display="http://test1.boxingtong.net:5222/token/loginPower" tooltip="http://test1.boxingtong.net:5222/token/loginPower"/>
     <hyperlink ref="E3" r:id="rId2" display="http://test1.boxingtong.net:5222/analyse/dashboard/queryActiveStatistics" tooltip="http://test1.boxingtong.net:5222/analyse/dashboard/queryActiveStatistics"/>
     <hyperlink ref="E4" r:id="rId3" display="http://test1.boxingtong.net:5222/analyse/dashboard/queryTraffic" tooltip="http://test1.boxingtong.net:5222/analyse/dashboard/queryTraffic"/>
-    <hyperlink ref="E5" r:id="rId4" display="http://test1.boxingtong.net:5222/analyse/dashboard/queryTrafficAv" tooltip="http://test1.boxingtong.net:5222/analyse/dashboard/queryTrafficAv"/>
+    <hyperlink ref="E5" r:id="rId4" display="http://test1.boxingtong.net:5222/analyse/dashboard/queryTrafficAvg" tooltip="http://test1.boxingtong.net:5222/analyse/dashboard/queryTrafficAvg"/>
     <hyperlink ref="E6" r:id="rId5" display="http://test1.boxingtong.net:5222/analyse/dashboard/queryOrderMoney" tooltip="http://test1.boxingtong.net:5222/analyse/dashboard/queryOrderMoney"/>
     <hyperlink ref="E7" r:id="rId6" display="http://test1.boxingtong.net:5222/analyse/dashboard/queryMoney" tooltip="http://test1.boxingtong.net:5222/analyse/dashboard/queryMoney"/>
     <hyperlink ref="E8" r:id="rId7" display="http://test1.boxingtong.net:5222/analyse/dashboard/newUser" tooltip="http://test1.boxingtong.net:5222/analyse/dashboard/newUser"/>
@@ -1632,76 +1586,267 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="36" style="1" customWidth="1"/>
-    <col min="3" max="3" width="93.1111111111111" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.4444444444444" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1111111111111" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.8888888888889" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.4444444444444" style="1" customWidth="1"/>
+    <col min="7" max="7" width="44" style="1" customWidth="1"/>
+    <col min="8" max="8" width="39" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="60" customHeight="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" ht="86.4" spans="1:8">
+      <c r="A2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" ht="155" customHeight="1" spans="1:2">
-      <c r="A2" t="s">
+    <row r="3" ht="86.4" spans="1:8">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>47</v>
+      <c r="D3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="3" ht="118" customHeight="1" spans="1:2">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="4" ht="86.4" spans="1:8">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="4" ht="97" customHeight="1" spans="1:2">
-      <c r="A4" t="s">
+    <row r="5" ht="86.4" spans="1:8">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>51</v>
-      </c>
     </row>
-    <row r="5" ht="135" customHeight="1" spans="2:2">
-      <c r="B5" s="2" t="s">
-        <v>52</v>
+    <row r="6" ht="86.4" spans="1:8">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" ht="86.4" spans="1:8">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" ht="86.4" spans="1:8">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" ht="86.4" spans="1:8">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="http://test1.boxingtong.net:9001/reward/selectRewardRecordList"/>
+    <hyperlink ref="E4" r:id="rId2" display="http://test1.boxingtong.net:9001/account/getVIPPopup"/>
+    <hyperlink ref="E5" r:id="rId3" display="http://test1.boxingtong.net:8001/banner/selectBanner"/>
+    <hyperlink ref="E6" r:id="rId4" display="http://test1.boxingtong.net:8001/consume/queryCurrentUsage" tooltip="http://test1.boxingtong.net:8001/consume/queryCurrentUsage"/>
+    <hyperlink ref="E8" r:id="rId5" display="http://test1.boxingtong.net:8001/banner/selectHomePopup"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>